<commit_message>
Better UI and upfront reports
</commit_message>
<xml_diff>
--- a/spull-band-finances.xlsx
+++ b/spull-band-finances.xlsx
@@ -10,6 +10,9 @@
     <sheet name="Cost Categories" sheetId="5" r:id="rId5"/>
     <sheet name="Individual Food Expenses" sheetId="6" r:id="rId6"/>
     <sheet name="Gig Profitability" sheetId="7" r:id="rId7"/>
+    <sheet name="Member Expense Breakdown" sheetId="8" r:id="rId8"/>
+    <sheet name="Upfront Payments" sheetId="9" r:id="rId9"/>
+    <sheet name="Payment Summary" sheetId="10" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -418,7 +421,7 @@
         <v>Generated:</v>
       </c>
       <c r="B2" t="str">
-        <v>9/15/2025 8:34:33 PM</v>
+        <v>9/15/2025 9:00:29 PM</v>
       </c>
     </row>
     <row r="4">
@@ -588,6 +591,273 @@
   </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:B28"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Member</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Total Paid Upfront (€)</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Total Expense Share (€)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Net Payment Impact (€)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Income (€)</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Final Balance (€)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Final + BTW (€)</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Max</v>
+      </c>
+      <c r="B2" t="str">
+        <v>140.30</v>
+      </c>
+      <c r="C2" t="str">
+        <v>56.52</v>
+      </c>
+      <c r="D2" t="str">
+        <v>83.78</v>
+      </c>
+      <c r="E2" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F2" t="str">
+        <v>236.72</v>
+      </c>
+      <c r="G2" t="str">
+        <v>258.02</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Naut</v>
+      </c>
+      <c r="B3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C3" t="str">
+        <v>56.52</v>
+      </c>
+      <c r="D3" t="str">
+        <v>-56.52</v>
+      </c>
+      <c r="E3" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F3" t="str">
+        <v>96.42</v>
+      </c>
+      <c r="G3" t="str">
+        <v>105.10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Filip</v>
+      </c>
+      <c r="B4" t="str">
+        <v>60.00</v>
+      </c>
+      <c r="C4" t="str">
+        <v>43.52</v>
+      </c>
+      <c r="D4" t="str">
+        <v>16.48</v>
+      </c>
+      <c r="E4" t="str">
+        <v>76.47</v>
+      </c>
+      <c r="F4" t="str">
+        <v>92.95</v>
+      </c>
+      <c r="G4" t="str">
+        <v>101.31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Dani</v>
+      </c>
+      <c r="B5" t="str">
+        <v>71.00</v>
+      </c>
+      <c r="C5" t="str">
+        <v>56.52</v>
+      </c>
+      <c r="D5" t="str">
+        <v>14.48</v>
+      </c>
+      <c r="E5" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F5" t="str">
+        <v>167.42</v>
+      </c>
+      <c r="G5" t="str">
+        <v>182.49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Pedro</v>
+      </c>
+      <c r="B6" t="str">
+        <v>45.70</v>
+      </c>
+      <c r="C6" t="str">
+        <v>43.52</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2.18</v>
+      </c>
+      <c r="E6" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F6" t="str">
+        <v>155.12</v>
+      </c>
+      <c r="G6" t="str">
+        <v>169.08</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Roman</v>
+      </c>
+      <c r="B7" t="str">
+        <v>9.62</v>
+      </c>
+      <c r="C7" t="str">
+        <v>43.52</v>
+      </c>
+      <c r="D7" t="str">
+        <v>-33.90</v>
+      </c>
+      <c r="E7" t="str">
+        <v>76.47</v>
+      </c>
+      <c r="F7" t="str">
+        <v>42.57</v>
+      </c>
+      <c r="G7" t="str">
+        <v>46.40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Frans</v>
+      </c>
+      <c r="B8" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C8" t="str">
+        <v>56.52</v>
+      </c>
+      <c r="D8" t="str">
+        <v>-56.52</v>
+      </c>
+      <c r="E8" t="str">
+        <v>76.47</v>
+      </c>
+      <c r="F8" t="str">
+        <v>19.95</v>
+      </c>
+      <c r="G8" t="str">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Steve</v>
+      </c>
+      <c r="B9" t="str">
+        <v>42.60</v>
+      </c>
+      <c r="C9" t="str">
+        <v>43.52</v>
+      </c>
+      <c r="D9" t="str">
+        <v>-0.92</v>
+      </c>
+      <c r="E9" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F9" t="str">
+        <v>152.02</v>
+      </c>
+      <c r="G9" t="str">
+        <v>165.70</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Kimo</v>
+      </c>
+      <c r="B10" t="str">
+        <v>66.00</v>
+      </c>
+      <c r="C10" t="str">
+        <v>43.52</v>
+      </c>
+      <c r="D10" t="str">
+        <v>22.48</v>
+      </c>
+      <c r="E10" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F10" t="str">
+        <v>175.42</v>
+      </c>
+      <c r="G10" t="str">
+        <v>191.21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Bandpot</v>
+      </c>
+      <c r="B11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C11" t="str">
+        <v>43.52</v>
+      </c>
+      <c r="D11" t="str">
+        <v>-43.52</v>
+      </c>
+      <c r="E11" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="F11" t="str">
+        <v>109.42</v>
+      </c>
+      <c r="G11" t="str">
+        <v>119.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1619,4 +1889,781 @@
     <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Member</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Food Individual (€)</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Travel Equal (€)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Travel Group (€)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Advertisement (€)</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Other (€)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Paid Out Total (€)</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Net Expense Share (€)</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Income (€)</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Net Balance (€)</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Net + BTW (€)</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Max</v>
+      </c>
+      <c r="B2" t="str">
+        <v>13.00</v>
+      </c>
+      <c r="C2" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D2" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E2" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F2" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G2" t="str">
+        <v>140.30</v>
+      </c>
+      <c r="H2" t="str">
+        <v>57.31</v>
+      </c>
+      <c r="I2" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J2" t="str">
+        <v>236.72</v>
+      </c>
+      <c r="K2" t="str">
+        <v>258.02</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Naut</v>
+      </c>
+      <c r="B3" t="str">
+        <v>13.00</v>
+      </c>
+      <c r="C3" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E3" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H3" t="str">
+        <v>57.31</v>
+      </c>
+      <c r="I3" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J3" t="str">
+        <v>96.42</v>
+      </c>
+      <c r="K3" t="str">
+        <v>105.10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Filip</v>
+      </c>
+      <c r="B4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C4" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E4" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G4" t="str">
+        <v>60.00</v>
+      </c>
+      <c r="H4" t="str">
+        <v>44.31</v>
+      </c>
+      <c r="I4" t="str">
+        <v>76.47</v>
+      </c>
+      <c r="J4" t="str">
+        <v>92.95</v>
+      </c>
+      <c r="K4" t="str">
+        <v>101.31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Dani</v>
+      </c>
+      <c r="B5" t="str">
+        <v>13.00</v>
+      </c>
+      <c r="C5" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D5" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E5" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F5" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G5" t="str">
+        <v>71.00</v>
+      </c>
+      <c r="H5" t="str">
+        <v>57.31</v>
+      </c>
+      <c r="I5" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J5" t="str">
+        <v>167.42</v>
+      </c>
+      <c r="K5" t="str">
+        <v>182.49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Pedro</v>
+      </c>
+      <c r="B6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C6" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E6" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G6" t="str">
+        <v>45.70</v>
+      </c>
+      <c r="H6" t="str">
+        <v>44.31</v>
+      </c>
+      <c r="I6" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J6" t="str">
+        <v>155.12</v>
+      </c>
+      <c r="K6" t="str">
+        <v>169.08</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Roman</v>
+      </c>
+      <c r="B7" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C7" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D7" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E7" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F7" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G7" t="str">
+        <v>9.62</v>
+      </c>
+      <c r="H7" t="str">
+        <v>44.31</v>
+      </c>
+      <c r="I7" t="str">
+        <v>76.47</v>
+      </c>
+      <c r="J7" t="str">
+        <v>42.57</v>
+      </c>
+      <c r="K7" t="str">
+        <v>46.40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Frans</v>
+      </c>
+      <c r="B8" t="str">
+        <v>13.00</v>
+      </c>
+      <c r="C8" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D8" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F8" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G8" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H8" t="str">
+        <v>57.31</v>
+      </c>
+      <c r="I8" t="str">
+        <v>76.47</v>
+      </c>
+      <c r="J8" t="str">
+        <v>19.95</v>
+      </c>
+      <c r="K8" t="str">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Steve</v>
+      </c>
+      <c r="B9" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C9" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D9" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F9" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G9" t="str">
+        <v>42.60</v>
+      </c>
+      <c r="H9" t="str">
+        <v>44.31</v>
+      </c>
+      <c r="I9" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J9" t="str">
+        <v>152.02</v>
+      </c>
+      <c r="K9" t="str">
+        <v>165.70</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Kimo</v>
+      </c>
+      <c r="B10" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C10" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D10" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E10" t="str">
+        <v>7.89</v>
+      </c>
+      <c r="F10" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G10" t="str">
+        <v>66.00</v>
+      </c>
+      <c r="H10" t="str">
+        <v>44.31</v>
+      </c>
+      <c r="I10" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J10" t="str">
+        <v>175.42</v>
+      </c>
+      <c r="K10" t="str">
+        <v>191.21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Bandpot</v>
+      </c>
+      <c r="B11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="C11" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="D11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H11" t="str">
+        <v>36.42</v>
+      </c>
+      <c r="I11" t="str">
+        <v>152.94</v>
+      </c>
+      <c r="J11" t="str">
+        <v>109.42</v>
+      </c>
+      <c r="K11" t="str">
+        <v>119.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:K11"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Member</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Expense Type</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Amount Paid (€)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Associated Gigs</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Date Added</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Split Among</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Member Share (€)</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Steve</v>
+      </c>
+      <c r="B2" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Car travel for Delft: 121km @ €0.20/km</v>
+      </c>
+      <c r="D2" t="str">
+        <v>24.20</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Delft</v>
+      </c>
+      <c r="F2" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G2" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Kimo</v>
+      </c>
+      <c r="B3" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Car travel for Delft: 130km @ €0.20/km</v>
+      </c>
+      <c r="D3" t="str">
+        <v>26.00</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Delft</v>
+      </c>
+      <c r="F3" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G3" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H3" t="str">
+        <v>2.60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Max</v>
+      </c>
+      <c r="B4" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Car travel for Delft: 140km @ €0.20/km</v>
+      </c>
+      <c r="D4" t="str">
+        <v>28.00</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Delft</v>
+      </c>
+      <c r="F4" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G4" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H4" t="str">
+        <v>2.80</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Pedro</v>
+      </c>
+      <c r="B5" t="str">
+        <v>general-travel</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Travel for Delft: Train</v>
+      </c>
+      <c r="D5" t="str">
+        <v>31.40</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Delft</v>
+      </c>
+      <c r="F5" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G5" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H5" t="str">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Max</v>
+      </c>
+      <c r="B6" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Car travel for Camping: 230km @ €0.20/km</v>
+      </c>
+      <c r="D6" t="str">
+        <v>46.00</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F6" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G6" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H6" t="str">
+        <v>4.60</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Steve</v>
+      </c>
+      <c r="B7" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Car travel for Camping: 92km @ €0.20/km</v>
+      </c>
+      <c r="D7" t="str">
+        <v>18.40</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F7" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G7" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H7" t="str">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Kimo</v>
+      </c>
+      <c r="B8" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Car travel for Camping: 200km @ €0.20/km</v>
+      </c>
+      <c r="D8" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F8" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G8" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H8" t="str">
+        <v>4.00</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Pedro</v>
+      </c>
+      <c r="B9" t="str">
+        <v>general-travel</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Travel for Camping: Train</v>
+      </c>
+      <c r="D9" t="str">
+        <v>14.30</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F9" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G9" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H9" t="str">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Roman</v>
+      </c>
+      <c r="B10" t="str">
+        <v>general-travel</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Travel for Camping: Train</v>
+      </c>
+      <c r="D10" t="str">
+        <v>9.62</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F10" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G10" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H10" t="str">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Max</v>
+      </c>
+      <c r="B11" t="str">
+        <v>parking</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Parking for Camping: Parking camping</v>
+      </c>
+      <c r="D11" t="str">
+        <v>9.50</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F11" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G11" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H11" t="str">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Max</v>
+      </c>
+      <c r="B12" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Car travel for Camping: Fixed amount</v>
+      </c>
+      <c r="D12" t="str">
+        <v>56.80</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F12" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G12" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H12" t="str">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Filip</v>
+      </c>
+      <c r="B13" t="str">
+        <v>car-travel</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Car travel for Camping: Fixed amount</v>
+      </c>
+      <c r="D13" t="str">
+        <v>60.00</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Camping</v>
+      </c>
+      <c r="F13" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G13" t="str">
+        <v>10 members (equal split)</v>
+      </c>
+      <c r="H13" t="str">
+        <v>6.00</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Dani</v>
+      </c>
+      <c r="B14" t="str">
+        <v>advertisement</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Advertisement for Delft, Camping: Ads</v>
+      </c>
+      <c r="D14" t="str">
+        <v>71.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Delft; Camping</v>
+      </c>
+      <c r="F14" t="str">
+        <v>9/15/2025</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Max, Naut, Filip, Dani, Pedro, Roman, Frans, Steve, Kimo</v>
+      </c>
+      <c r="H14" t="str">
+        <v>7.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>